<commit_message>
first values to Singapore archetypes database
first values to Singapore archetypes database (work in progress)
</commit_message>
<xml_diff>
--- a/cea/databases/archetypes/construction_properties_SIN.xlsx
+++ b/cea/databases/archetypes/construction_properties_SIN.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jimeno\Documents\CEAforArcGIS\cea\databases\archetypes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel\Documents\GitHub\CEAforArcGIS\cea\databases\archetypes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="56">
   <si>
     <t>Code</t>
   </si>
@@ -183,6 +183,21 @@
   </si>
   <si>
     <t>building_use</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>T2</t>
+  </si>
+  <si>
+    <t>T7</t>
+  </si>
+  <si>
+    <t>T6</t>
+  </si>
+  <si>
+    <t>T0</t>
   </si>
 </sst>
 </file>
@@ -1076,24 +1091,24 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G23" sqref="G23"/>
+      <selection pane="bottomRight" activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.9296875" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.53125" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.53125" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="7.1328125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="10.86328125" style="4" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="11.1328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="12" width="12.3984375" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.1328125" style="1"/>
+    <col min="1" max="1" width="12" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="7.140625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" style="4" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="12.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>50</v>
       </c>
@@ -1131,7 +1146,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>18</v>
       </c>
@@ -1142,15 +1157,21 @@
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
+      <c r="G2" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
+      <c r="J2" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="L2" s="3"/>
       <c r="N2" s="12"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>19</v>
       </c>
@@ -1161,14 +1182,20 @@
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
+      <c r="G3" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
+      <c r="J3" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>20</v>
       </c>
@@ -1179,14 +1206,18 @@
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
+      <c r="G4" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
+      <c r="J4" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>21</v>
       </c>
@@ -1196,15 +1227,27 @@
         <v>48</v>
       </c>
       <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
+      <c r="F5" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="L5" s="3"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>22</v>
       </c>
@@ -1215,14 +1258,20 @@
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
+      <c r="G6" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
+      <c r="J6" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="L6" s="3"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>32</v>
       </c>
@@ -1233,14 +1282,18 @@
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
+      <c r="G7" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
+      <c r="J7" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>23</v>
       </c>
@@ -1251,14 +1304,20 @@
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
+      <c r="G8" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
+      <c r="J8" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="L8" s="3"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>24</v>
       </c>
@@ -1269,14 +1328,18 @@
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
+      <c r="G9" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
+      <c r="J9" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>25</v>
       </c>
@@ -1287,14 +1350,20 @@
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
+      <c r="G10" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
+      <c r="J10" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="L10" s="3"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>26</v>
       </c>
@@ -1305,14 +1374,18 @@
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
+      <c r="G11" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
+      <c r="J11" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>27</v>
       </c>
@@ -1323,14 +1396,20 @@
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
+      <c r="G12" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
+      <c r="J12" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="L12" s="3"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>28</v>
       </c>
@@ -1341,14 +1420,18 @@
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
+      <c r="G13" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
+      <c r="J13" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>29</v>
       </c>
@@ -1359,14 +1442,18 @@
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
+      <c r="G14" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
+      <c r="J14" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>30</v>
       </c>
@@ -1377,14 +1464,18 @@
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
+      <c r="G15" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
+      <c r="J15" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>31</v>
       </c>
@@ -1395,14 +1486,18 @@
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
+      <c r="G16" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
+      <c r="J16" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>41</v>
       </c>
@@ -1412,15 +1507,23 @@
         <v>48</v>
       </c>
       <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
+      <c r="F17" s="3">
+        <v>0.11</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
+      <c r="J17" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="L17" s="3"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>42</v>
       </c>
@@ -1431,14 +1534,20 @@
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
+      <c r="G18" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
+      <c r="J18" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="L18" s="3"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>43</v>
       </c>
@@ -1449,11 +1558,17 @@
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
+      <c r="G19" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
+      <c r="J19" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="L19" s="3"/>
     </row>
   </sheetData>
@@ -1470,23 +1585,23 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2:A19"/>
+      <selection pane="bottomRight" activeCell="E2" sqref="E2:E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.59765625" style="14" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" style="14" customWidth="1"/>
-    <col min="4" max="4" width="7.9296875" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="9.1328125" style="4"/>
-    <col min="7" max="7" width="9.86328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.86328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.265625" style="4" customWidth="1"/>
-    <col min="10" max="16384" width="9.1328125" style="1"/>
+    <col min="1" max="1" width="12.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" style="14" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" style="14" customWidth="1"/>
+    <col min="4" max="4" width="8" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="9.140625" style="4"/>
+    <col min="7" max="7" width="9.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" style="4" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>50</v>
       </c>
@@ -1515,7 +1630,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>18</v>
       </c>
@@ -1524,13 +1639,15 @@
       <c r="D2" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E2" s="3"/>
+      <c r="E2" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>19</v>
       </c>
@@ -1539,13 +1656,15 @@
       <c r="D3" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E3" s="3"/>
+      <c r="E3" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>20</v>
       </c>
@@ -1554,13 +1673,15 @@
       <c r="D4" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="3"/>
+      <c r="E4" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>21</v>
       </c>
@@ -1569,13 +1690,15 @@
       <c r="D5" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E5" s="3"/>
+      <c r="E5" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>22</v>
       </c>
@@ -1584,13 +1707,15 @@
       <c r="D6" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E6" s="3"/>
+      <c r="E6" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>32</v>
       </c>
@@ -1599,13 +1724,15 @@
       <c r="D7" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E7" s="3"/>
+      <c r="E7" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>23</v>
       </c>
@@ -1614,13 +1741,15 @@
       <c r="D8" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E8" s="3"/>
+      <c r="E8" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>24</v>
       </c>
@@ -1629,13 +1758,15 @@
       <c r="D9" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E9" s="3"/>
+      <c r="E9" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>25</v>
       </c>
@@ -1644,13 +1775,15 @@
       <c r="D10" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E10" s="3"/>
+      <c r="E10" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>26</v>
       </c>
@@ -1659,13 +1792,15 @@
       <c r="D11" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E11" s="3"/>
+      <c r="E11" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>27</v>
       </c>
@@ -1674,13 +1809,15 @@
       <c r="D12" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E12" s="3"/>
+      <c r="E12" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>28</v>
       </c>
@@ -1689,13 +1826,15 @@
       <c r="D13" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E13" s="3"/>
+      <c r="E13" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>29</v>
       </c>
@@ -1704,13 +1843,15 @@
       <c r="D14" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E14" s="3"/>
+      <c r="E14" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>30</v>
       </c>
@@ -1719,13 +1860,15 @@
       <c r="D15" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E15" s="3"/>
+      <c r="E15" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>31</v>
       </c>
@@ -1734,13 +1877,15 @@
       <c r="D16" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E16" s="3"/>
+      <c r="E16" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>41</v>
       </c>
@@ -1749,13 +1894,15 @@
       <c r="D17" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E17" s="3"/>
+      <c r="E17" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>42</v>
       </c>
@@ -1764,13 +1911,15 @@
       <c r="D18" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E18" s="3"/>
+      <c r="E18" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>43</v>
       </c>
@@ -1779,7 +1928,9 @@
       <c r="D19" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E19" s="3"/>
+      <c r="E19" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
@@ -1799,18 +1950,18 @@
       <selection activeCell="A2" sqref="A2:A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.3984375" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.86328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.3984375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.86328125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="12" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.73046875" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.1328125" style="1"/>
+    <col min="6" max="6" width="9.7109375" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1830,7 +1981,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>18</v>
       </c>
@@ -1840,7 +1991,7 @@
       <c r="E2" s="5"/>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>19</v>
       </c>
@@ -1850,7 +2001,7 @@
       <c r="E3" s="5"/>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>20</v>
       </c>
@@ -1860,7 +2011,7 @@
       <c r="E4" s="5"/>
       <c r="F4" s="9"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>21</v>
       </c>
@@ -1870,7 +2021,7 @@
       <c r="E5" s="5"/>
       <c r="F5" s="9"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>22</v>
       </c>
@@ -1880,7 +2031,7 @@
       <c r="E6" s="5"/>
       <c r="F6" s="9"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>32</v>
       </c>
@@ -1890,7 +2041,7 @@
       <c r="E7" s="5"/>
       <c r="F7" s="9"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>23</v>
       </c>
@@ -1900,7 +2051,7 @@
       <c r="E8" s="5"/>
       <c r="F8" s="9"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>24</v>
       </c>
@@ -1910,7 +2061,7 @@
       <c r="E9" s="5"/>
       <c r="F9" s="9"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>25</v>
       </c>
@@ -1920,7 +2071,7 @@
       <c r="E10" s="5"/>
       <c r="F10" s="9"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>26</v>
       </c>
@@ -1930,7 +2081,7 @@
       <c r="E11" s="5"/>
       <c r="F11" s="9"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>27</v>
       </c>
@@ -1940,7 +2091,7 @@
       <c r="E12" s="5"/>
       <c r="F12" s="9"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>28</v>
       </c>
@@ -1950,7 +2101,7 @@
       <c r="E13" s="5"/>
       <c r="F13" s="9"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>29</v>
       </c>
@@ -1960,7 +2111,7 @@
       <c r="E14" s="5"/>
       <c r="F14" s="9"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>30</v>
       </c>
@@ -1970,7 +2121,7 @@
       <c r="E15" s="5"/>
       <c r="F15" s="9"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>31</v>
       </c>
@@ -1980,7 +2131,7 @@
       <c r="E16" s="5"/>
       <c r="F16" s="9"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>41</v>
       </c>
@@ -1990,7 +2141,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="9"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>42</v>
       </c>
@@ -2000,7 +2151,7 @@
       <c r="E18" s="5"/>
       <c r="F18" s="9"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>43</v>
       </c>
@@ -2024,21 +2175,21 @@
       <selection activeCell="D2" sqref="D2:J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.3984375" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="8.3984375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.265625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.1328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.1328125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9.73046875" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.1328125" style="1"/>
+    <col min="1" max="1" width="15.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="8.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -2070,7 +2221,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>18</v>
       </c>
@@ -2088,7 +2239,7 @@
       <c r="I2" s="9"/>
       <c r="J2" s="9"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>19</v>
       </c>
@@ -2106,7 +2257,7 @@
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>20</v>
       </c>
@@ -2124,7 +2275,7 @@
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>21</v>
       </c>
@@ -2142,7 +2293,7 @@
       <c r="I5" s="9"/>
       <c r="J5" s="9"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>22</v>
       </c>
@@ -2160,7 +2311,7 @@
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>32</v>
       </c>
@@ -2178,7 +2329,7 @@
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>23</v>
       </c>
@@ -2196,7 +2347,7 @@
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>24</v>
       </c>
@@ -2214,7 +2365,7 @@
       <c r="I9" s="9"/>
       <c r="J9" s="9"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>25</v>
       </c>
@@ -2232,7 +2383,7 @@
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>26</v>
       </c>
@@ -2250,7 +2401,7 @@
       <c r="I11" s="9"/>
       <c r="J11" s="9"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>27</v>
       </c>
@@ -2268,7 +2419,7 @@
       <c r="I12" s="9"/>
       <c r="J12" s="9"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>28</v>
       </c>
@@ -2286,7 +2437,7 @@
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>29</v>
       </c>
@@ -2304,7 +2455,7 @@
       <c r="I14" s="9"/>
       <c r="J14" s="9"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>30</v>
       </c>
@@ -2322,7 +2473,7 @@
       <c r="I15" s="9"/>
       <c r="J15" s="9"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>31</v>
       </c>
@@ -2340,7 +2491,7 @@
       <c r="I16" s="9"/>
       <c r="J16" s="9"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>41</v>
       </c>
@@ -2360,7 +2511,7 @@
       <c r="I17" s="9"/>
       <c r="J17" s="9"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>42</v>
       </c>
@@ -2378,7 +2529,7 @@
       <c r="I18" s="9"/>
       <c r="J18" s="9"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>43</v>
       </c>
@@ -2396,7 +2547,7 @@
       <c r="I19" s="9"/>
       <c r="J19" s="9"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G22" s="13"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add Hs to Singapore archetypes
add Hs
</commit_message>
<xml_diff>
--- a/cea/databases/archetypes/construction_properties_SIN.xlsx
+++ b/cea/databases/archetypes/construction_properties_SIN.xlsx
@@ -1091,7 +1091,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G19" sqref="G19"/>
+      <selection pane="bottomRight" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1155,7 +1155,9 @@
       <c r="D2" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E2" s="3"/>
+      <c r="E2" s="3">
+        <v>0.25</v>
+      </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3" t="s">
         <v>52</v>
@@ -1180,7 +1182,9 @@
       <c r="D3" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E3" s="3"/>
+      <c r="E3" s="3">
+        <v>0.25</v>
+      </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3" t="s">
         <v>52</v>
@@ -1204,7 +1208,9 @@
       <c r="D4" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="3"/>
+      <c r="E4" s="3">
+        <v>0.84</v>
+      </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3" t="s">
         <v>52</v>
@@ -1226,7 +1232,9 @@
       <c r="D5" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E5" s="3"/>
+      <c r="E5" s="3">
+        <v>0.84</v>
+      </c>
       <c r="F5" s="3">
         <v>0.35</v>
       </c>
@@ -1256,7 +1264,9 @@
       <c r="D6" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E6" s="3"/>
+      <c r="E6" s="3">
+        <v>0.84</v>
+      </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3" t="s">
         <v>52</v>
@@ -1280,7 +1290,9 @@
       <c r="D7" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E7" s="3"/>
+      <c r="E7" s="3">
+        <v>0.84</v>
+      </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3" t="s">
         <v>52</v>
@@ -1302,7 +1314,9 @@
       <c r="D8" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E8" s="3"/>
+      <c r="E8" s="3">
+        <v>0.84</v>
+      </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3" t="s">
         <v>52</v>
@@ -1326,7 +1340,9 @@
       <c r="D9" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E9" s="3"/>
+      <c r="E9" s="3">
+        <v>0.7</v>
+      </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3" t="s">
         <v>52</v>
@@ -1348,7 +1364,9 @@
       <c r="D10" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E10" s="3"/>
+      <c r="E10" s="3">
+        <v>0.67</v>
+      </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3" t="s">
         <v>52</v>
@@ -1372,7 +1390,9 @@
       <c r="D11" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E11" s="3"/>
+      <c r="E11" s="3">
+        <v>0.84</v>
+      </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3" t="s">
         <v>52</v>
@@ -1394,7 +1414,9 @@
       <c r="D12" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E12" s="3"/>
+      <c r="E12" s="3">
+        <v>0.67</v>
+      </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3" t="s">
         <v>52</v>
@@ -1418,7 +1440,9 @@
       <c r="D13" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E13" s="3"/>
+      <c r="E13" s="3">
+        <v>0</v>
+      </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3" t="s">
         <v>52</v>
@@ -1440,7 +1464,9 @@
       <c r="D14" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E14" s="3"/>
+      <c r="E14" s="3">
+        <v>1</v>
+      </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3" t="s">
         <v>52</v>
@@ -1462,7 +1488,9 @@
       <c r="D15" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E15" s="3"/>
+      <c r="E15" s="3">
+        <v>0</v>
+      </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3" t="s">
         <v>52</v>
@@ -1484,7 +1512,9 @@
       <c r="D16" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E16" s="3"/>
+      <c r="E16" s="3">
+        <v>1</v>
+      </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3" t="s">
         <v>52</v>
@@ -1506,7 +1536,9 @@
       <c r="D17" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E17" s="3"/>
+      <c r="E17" s="3">
+        <v>0.67</v>
+      </c>
       <c r="F17" s="3">
         <v>0.11</v>
       </c>
@@ -1532,7 +1564,9 @@
       <c r="D18" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E18" s="3"/>
+      <c r="E18" s="3">
+        <v>0.67</v>
+      </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3" t="s">
         <v>52</v>
@@ -1556,7 +1590,9 @@
       <c r="D19" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E19" s="3"/>
+      <c r="E19" s="3">
+        <v>0.67</v>
+      </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3" t="s">
         <v>52</v>

</xml_diff>

<commit_message>
Singapore Archetypes (excl. shading systems)
- added custom envelope systems (windows, walls)
- added custom ventilation control (mechanical w/o night flushing)
</commit_message>
<xml_diff>
--- a/cea/databases/archetypes/construction_properties_SIN.xlsx
+++ b/cea/databases/archetypes/construction_properties_SIN.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16140" tabRatio="785"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="14370" windowHeight="11115" tabRatio="785"/>
   </bookViews>
   <sheets>
     <sheet name="ARCHITECTURE" sheetId="3" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="61">
   <si>
     <t>Code</t>
   </si>
@@ -198,6 +198,21 @@
   </si>
   <si>
     <t>T0</t>
+  </si>
+  <si>
+    <t>T3</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>T8</t>
+  </si>
+  <si>
+    <t>T9</t>
+  </si>
+  <si>
+    <t>T10</t>
   </si>
 </sst>
 </file>
@@ -724,7 +739,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -735,10 +750,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -1091,14 +1102,14 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E12" sqref="E12"/>
+      <selection pane="bottomRight" activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" style="13" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.28515625" style="4" customWidth="1"/>
     <col min="5" max="5" width="7.140625" style="4" customWidth="1"/>
     <col min="6" max="6" width="10.85546875" style="4" customWidth="1"/>
@@ -1109,61 +1120,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
       <c r="D2" s="2" t="s">
         <v>48</v>
       </c>
       <c r="E2" s="3">
         <v>0.25</v>
       </c>
-      <c r="F2" s="3"/>
+      <c r="F2" s="3">
+        <v>0.28999999999999998</v>
+      </c>
       <c r="G2" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
+      <c r="H2" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>58</v>
+      </c>
       <c r="J2" s="3" t="s">
         <v>53</v>
       </c>
@@ -1171,26 +1188,32 @@
         <v>52</v>
       </c>
       <c r="L2" s="3"/>
-      <c r="N2" s="12"/>
+      <c r="N2" s="11"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
       <c r="D3" s="2" t="s">
         <v>48</v>
       </c>
       <c r="E3" s="3">
         <v>0.25</v>
       </c>
-      <c r="F3" s="3"/>
+      <c r="F3" s="3">
+        <v>0.28999999999999998</v>
+      </c>
       <c r="G3" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
+      <c r="H3" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>58</v>
+      </c>
       <c r="J3" s="3" t="s">
         <v>53</v>
       </c>
@@ -1200,35 +1223,43 @@
       <c r="L3" s="3"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
       <c r="D4" s="2" t="s">
         <v>48</v>
       </c>
       <c r="E4" s="3">
         <v>0.84</v>
       </c>
-      <c r="F4" s="3"/>
+      <c r="F4" s="3">
+        <v>0.35</v>
+      </c>
       <c r="G4" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
+      <c r="H4" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>60</v>
+      </c>
       <c r="J4" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="K4" s="3"/>
+      <c r="K4" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="L4" s="3"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
       <c r="D5" s="2" t="s">
         <v>48</v>
       </c>
@@ -1245,7 +1276,7 @@
         <v>51</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>53</v>
@@ -1256,23 +1287,29 @@
       <c r="L5" s="3"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
       <c r="D6" s="2" t="s">
         <v>48</v>
       </c>
       <c r="E6" s="3">
         <v>0.84</v>
       </c>
-      <c r="F6" s="3"/>
+      <c r="F6" s="3">
+        <v>0.35</v>
+      </c>
       <c r="G6" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
+      <c r="H6" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>60</v>
+      </c>
       <c r="J6" s="3" t="s">
         <v>53</v>
       </c>
@@ -1282,47 +1319,61 @@
       <c r="L6" s="3"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
       <c r="D7" s="2" t="s">
         <v>48</v>
       </c>
       <c r="E7" s="3">
         <v>0.84</v>
       </c>
-      <c r="F7" s="3"/>
+      <c r="F7" s="3">
+        <v>0</v>
+      </c>
       <c r="G7" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
+      <c r="H7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>60</v>
+      </c>
       <c r="J7" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="K7" s="3"/>
+      <c r="K7" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="L7" s="3"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
       <c r="D8" s="2" t="s">
         <v>48</v>
       </c>
       <c r="E8" s="3">
         <v>0.84</v>
       </c>
-      <c r="F8" s="3"/>
+      <c r="F8" s="3">
+        <v>0.35</v>
+      </c>
       <c r="G8" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
+      <c r="H8" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>60</v>
+      </c>
       <c r="J8" s="3" t="s">
         <v>53</v>
       </c>
@@ -1332,47 +1383,61 @@
       <c r="L8" s="3"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
       <c r="D9" s="2" t="s">
         <v>48</v>
       </c>
       <c r="E9" s="3">
         <v>0.7</v>
       </c>
-      <c r="F9" s="3"/>
+      <c r="F9" s="3">
+        <v>0.1</v>
+      </c>
       <c r="G9" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
+      <c r="H9" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>60</v>
+      </c>
       <c r="J9" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="K9" s="3"/>
+      <c r="K9" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="L9" s="3"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
       <c r="D10" s="2" t="s">
         <v>48</v>
       </c>
       <c r="E10" s="3">
         <v>0.67</v>
       </c>
-      <c r="F10" s="3"/>
+      <c r="F10" s="3">
+        <v>0.35</v>
+      </c>
       <c r="G10" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
+      <c r="H10" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>59</v>
+      </c>
       <c r="J10" s="3" t="s">
         <v>53</v>
       </c>
@@ -1382,47 +1447,61 @@
       <c r="L10" s="3"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
       <c r="D11" s="2" t="s">
         <v>48</v>
       </c>
       <c r="E11" s="3">
         <v>0.84</v>
       </c>
-      <c r="F11" s="3"/>
+      <c r="F11" s="3">
+        <v>0.35</v>
+      </c>
       <c r="G11" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
+      <c r="H11" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>60</v>
+      </c>
       <c r="J11" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="K11" s="3"/>
+      <c r="K11" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="L11" s="3"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
       <c r="D12" s="2" t="s">
         <v>48</v>
       </c>
       <c r="E12" s="3">
         <v>0.67</v>
       </c>
-      <c r="F12" s="3"/>
+      <c r="F12" s="3">
+        <v>0.35</v>
+      </c>
       <c r="G12" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
+      <c r="H12" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>59</v>
+      </c>
       <c r="J12" s="3" t="s">
         <v>53</v>
       </c>
@@ -1432,107 +1511,139 @@
       <c r="L12" s="3"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
       <c r="D13" s="2" t="s">
         <v>48</v>
       </c>
       <c r="E13" s="3">
         <v>0</v>
       </c>
-      <c r="F13" s="3"/>
+      <c r="F13" s="3">
+        <v>0.35</v>
+      </c>
       <c r="G13" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
+      <c r="H13" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>60</v>
+      </c>
       <c r="J13" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="K13" s="3"/>
+      <c r="K13" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="L13" s="3"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
       <c r="D14" s="2" t="s">
         <v>48</v>
       </c>
       <c r="E14" s="3">
         <v>1</v>
       </c>
-      <c r="F14" s="3"/>
+      <c r="F14" s="3">
+        <v>0</v>
+      </c>
       <c r="G14" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
+      <c r="H14" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>60</v>
+      </c>
       <c r="J14" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="K14" s="3"/>
+      <c r="K14" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="L14" s="3"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
       <c r="D15" s="2" t="s">
         <v>48</v>
       </c>
       <c r="E15" s="3">
         <v>0</v>
       </c>
-      <c r="F15" s="3"/>
+      <c r="F15" s="3">
+        <v>0.5</v>
+      </c>
       <c r="G15" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
+      <c r="H15" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="J15" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="K15" s="3"/>
+      <c r="K15" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="L15" s="3"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
       <c r="D16" s="2" t="s">
         <v>48</v>
       </c>
       <c r="E16" s="3">
         <v>1</v>
       </c>
-      <c r="F16" s="3"/>
+      <c r="F16" s="3">
+        <v>0</v>
+      </c>
       <c r="G16" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
+      <c r="H16" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="J16" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="K16" s="3"/>
+      <c r="K16" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="L16" s="3"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
       <c r="D17" s="2" t="s">
         <v>48</v>
       </c>
@@ -1540,13 +1651,17 @@
         <v>0.67</v>
       </c>
       <c r="F17" s="3">
-        <v>0.11</v>
+        <v>0.35</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
+      <c r="H17" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>59</v>
+      </c>
       <c r="J17" s="3" t="s">
         <v>53</v>
       </c>
@@ -1556,23 +1671,29 @@
       <c r="L17" s="3"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
       <c r="D18" s="2" t="s">
         <v>48</v>
       </c>
       <c r="E18" s="3">
         <v>0.67</v>
       </c>
-      <c r="F18" s="3"/>
+      <c r="F18" s="3">
+        <v>0.35</v>
+      </c>
       <c r="G18" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
+      <c r="H18" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>59</v>
+      </c>
       <c r="J18" s="3" t="s">
         <v>53</v>
       </c>
@@ -1582,23 +1703,29 @@
       <c r="L18" s="3"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
       <c r="D19" s="2" t="s">
         <v>48</v>
       </c>
       <c r="E19" s="3">
         <v>0.67</v>
       </c>
-      <c r="F19" s="3"/>
+      <c r="F19" s="3">
+        <v>0.35</v>
+      </c>
       <c r="G19" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
+      <c r="H19" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>59</v>
+      </c>
       <c r="J19" s="3" t="s">
         <v>53</v>
       </c>
@@ -1615,20 +1742,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I1048576"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E2" sqref="E2:E19"/>
+      <selection pane="bottomRight" activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" style="14" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" style="14" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" style="13" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" style="13" customWidth="1"/>
     <col min="4" max="4" width="8" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="9.140625" style="4"/>
     <col min="7" max="7" width="9.85546875" style="4" bestFit="1" customWidth="1"/>
@@ -1638,339 +1765,486 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="6" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
       <c r="D2" s="2" t="s">
         <v>48</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
+      <c r="F2" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
       <c r="D3" s="2" t="s">
         <v>48</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
+      <c r="F3" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
       <c r="D4" s="2" t="s">
         <v>48</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
+      <c r="F4" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
       <c r="D5" s="2" t="s">
         <v>48</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
+      <c r="F5" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
       <c r="D6" s="2" t="s">
         <v>48</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
+      <c r="F6" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
       <c r="D7" s="2" t="s">
         <v>48</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
+      <c r="F7" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
       <c r="D8" s="2" t="s">
         <v>48</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
+      <c r="F8" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
       <c r="D9" s="2" t="s">
         <v>48</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
+      <c r="F9" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
       <c r="D10" s="2" t="s">
         <v>48</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
+      <c r="F10" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
       <c r="D11" s="2" t="s">
         <v>48</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
+      <c r="F11" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
       <c r="D12" s="2" t="s">
         <v>48</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
+      <c r="F12" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
       <c r="D13" s="2" t="s">
         <v>48</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
+      <c r="F13" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
       <c r="D14" s="2" t="s">
         <v>48</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
+      <c r="F14" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
       <c r="D15" s="2" t="s">
         <v>48</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
+      <c r="F15" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
       <c r="D16" s="2" t="s">
         <v>48</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
+      <c r="F16" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
       <c r="D17" s="2" t="s">
         <v>48</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
+      <c r="F17" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
       <c r="D18" s="2" t="s">
         <v>48</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
+      <c r="F18" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
       <c r="D19" s="2" t="s">
         <v>48</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
+      <c r="F19" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="1048576" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H1048576" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1983,7 +2257,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A19"/>
+      <selection activeCell="F2" sqref="F2:F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1998,204 +2272,386 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="7" t="s">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="6"/>
+      <c r="B2" s="8">
+        <v>24</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="8">
+        <v>24</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" s="5">
+        <v>10</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="6"/>
+      <c r="B3" s="8">
+        <v>24</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="8">
+        <v>24</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F3" s="5">
+        <v>10</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="9"/>
+      <c r="B4" s="8">
+        <v>24</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="8">
+        <v>24</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F4" s="8">
+        <v>10</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="9"/>
+      <c r="B5" s="8">
+        <v>24</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="3">
+        <v>37</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F5" s="8">
+        <v>10</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="9"/>
+      <c r="B6" s="8">
+        <v>24</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" s="3">
+        <v>37</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F6" s="8">
+        <v>8</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="9"/>
+      <c r="B7" s="8">
+        <v>24</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" s="8">
+        <v>24</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F7" s="8">
+        <v>10</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="9"/>
+      <c r="B8" s="8">
+        <v>24</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" s="3">
+        <v>37</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F8" s="8">
+        <f t="shared" ref="F8" si="0">111*0.15+10*0.85</f>
+        <v>25.15</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="9"/>
+      <c r="B9" s="8">
+        <v>24</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="3">
+        <v>37</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F9" s="8">
+        <v>31</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="9"/>
+      <c r="B10" s="8">
+        <v>24</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" s="3">
+        <v>37</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F10" s="8">
+        <v>8</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="9"/>
+      <c r="B11" s="8">
+        <v>24</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" s="8">
+        <v>24</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F11" s="8">
+        <v>10</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="9"/>
+      <c r="B12" s="8">
+        <v>24</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="3">
+        <v>37</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F12" s="8">
+        <v>10</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="9"/>
+      <c r="B13" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F13" s="8">
+        <v>36</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="9"/>
+      <c r="B14" s="8">
+        <v>24</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" s="8">
+        <v>24</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F14" s="8">
+        <v>36</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="9"/>
+      <c r="B15" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F15" s="8">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="9"/>
+      <c r="B16" s="8">
+        <v>-5</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="8">
+        <v>-5</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F16" s="8">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="9"/>
+      <c r="B17" s="8">
+        <v>24</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" s="3">
+        <v>37</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F17" s="8">
+        <f>F9</f>
+        <v>31</v>
+      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="9"/>
+      <c r="B18" s="8">
+        <v>24</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" s="3">
+        <v>37</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F18" s="8">
+        <v>10</v>
+      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="9"/>
+      <c r="B19" s="8">
+        <v>24</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D19" s="3">
+        <v>37</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F19" s="8">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2208,7 +2664,7 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:J19"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2226,365 +2682,618 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="7" t="s">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B2" s="8">
         <v>70</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="8">
         <v>80</v>
       </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
+      <c r="D2" s="8">
+        <v>5.5</v>
+      </c>
+      <c r="E2" s="8">
+        <v>10.5</v>
+      </c>
+      <c r="F2" s="5">
+        <v>0</v>
+      </c>
+      <c r="G2" s="8">
+        <v>0</v>
+      </c>
+      <c r="H2" s="5">
+        <v>0</v>
+      </c>
+      <c r="I2" s="8">
+        <v>40</v>
+      </c>
+      <c r="J2" s="8">
+        <v>80</v>
+      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="5">
         <v>70</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="5">
         <v>80</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
+      <c r="D3" s="5">
+        <v>5.5</v>
+      </c>
+      <c r="E3" s="5">
+        <v>10.52</v>
+      </c>
+      <c r="F3" s="8">
+        <v>0</v>
+      </c>
+      <c r="G3" s="8">
+        <v>0</v>
+      </c>
+      <c r="H3" s="5">
+        <v>0</v>
+      </c>
+      <c r="I3" s="8">
+        <v>40</v>
+      </c>
+      <c r="J3" s="8">
+        <v>80</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="8">
         <v>70</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="8">
         <v>80</v>
       </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
+      <c r="D4" s="8">
+        <v>4.3</v>
+      </c>
+      <c r="E4" s="8">
+        <v>3.1</v>
+      </c>
+      <c r="F4" s="8">
+        <v>0</v>
+      </c>
+      <c r="G4" s="8">
+        <v>0</v>
+      </c>
+      <c r="H4" s="5">
+        <v>0</v>
+      </c>
+      <c r="I4" s="8">
+        <v>40</v>
+      </c>
+      <c r="J4" s="8">
+        <v>80</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="8">
         <v>70</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="8">
         <v>80</v>
       </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
+      <c r="D5" s="8">
+        <v>15</v>
+      </c>
+      <c r="E5" s="8">
+        <v>14</v>
+      </c>
+      <c r="F5" s="8">
+        <v>0</v>
+      </c>
+      <c r="G5" s="8">
+        <v>0</v>
+      </c>
+      <c r="H5" s="5">
+        <v>0</v>
+      </c>
+      <c r="I5" s="8">
+        <v>0</v>
+      </c>
+      <c r="J5" s="8">
+        <v>20</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="8">
         <v>70</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="8">
         <v>90</v>
       </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
+      <c r="D6" s="8">
+        <v>2</v>
+      </c>
+      <c r="E6" s="8">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="F6" s="8">
+        <v>0</v>
+      </c>
+      <c r="G6" s="8">
+        <v>0</v>
+      </c>
+      <c r="H6" s="5">
+        <v>0</v>
+      </c>
+      <c r="I6" s="8">
+        <v>2</v>
+      </c>
+      <c r="J6" s="8">
+        <v>4</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="8">
         <v>70</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="8">
         <v>80</v>
       </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
+      <c r="D7" s="8">
+        <v>5</v>
+      </c>
+      <c r="E7" s="8">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="F7" s="8">
+        <v>0</v>
+      </c>
+      <c r="G7" s="8">
+        <v>0</v>
+      </c>
+      <c r="H7" s="5">
+        <v>0</v>
+      </c>
+      <c r="I7" s="8">
+        <v>2</v>
+      </c>
+      <c r="J7" s="8">
+        <v>4</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="8">
         <v>73</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="8">
         <v>85</v>
       </c>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
+      <c r="D8" s="8">
+        <v>31.7</v>
+      </c>
+      <c r="E8" s="8">
+        <v>8.25</v>
+      </c>
+      <c r="F8" s="8">
+        <v>0</v>
+      </c>
+      <c r="G8" s="8">
+        <v>0</v>
+      </c>
+      <c r="H8" s="5">
+        <v>0</v>
+      </c>
+      <c r="I8" s="8">
+        <v>8</v>
+      </c>
+      <c r="J8" s="8">
+        <v>16</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9" s="8">
         <v>90</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="8">
         <v>170</v>
       </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
+      <c r="D9" s="8">
+        <v>20</v>
+      </c>
+      <c r="E9" s="8">
+        <v>14.7</v>
+      </c>
+      <c r="F9" s="8">
+        <v>16.5</v>
+      </c>
+      <c r="G9" s="8">
+        <v>0</v>
+      </c>
+      <c r="H9" s="5">
+        <v>0</v>
+      </c>
+      <c r="I9" s="8">
+        <v>10</v>
+      </c>
+      <c r="J9" s="8">
+        <v>20</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10" s="8">
         <v>70</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="8">
         <v>80</v>
       </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
+      <c r="D10" s="8">
+        <v>16</v>
+      </c>
+      <c r="E10" s="8">
+        <v>12</v>
+      </c>
+      <c r="F10" s="8">
+        <v>0</v>
+      </c>
+      <c r="G10" s="8">
+        <v>0</v>
+      </c>
+      <c r="H10" s="5">
+        <v>0</v>
+      </c>
+      <c r="I10" s="8">
+        <v>0</v>
+      </c>
+      <c r="J10" s="8">
+        <v>4</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B11" s="8">
         <v>70</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="8">
         <v>80</v>
       </c>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
+      <c r="D11" s="8">
+        <v>8</v>
+      </c>
+      <c r="E11" s="8">
+        <v>11</v>
+      </c>
+      <c r="F11" s="8">
+        <v>0</v>
+      </c>
+      <c r="G11" s="8">
+        <v>0</v>
+      </c>
+      <c r="H11" s="5">
+        <v>0</v>
+      </c>
+      <c r="I11" s="8">
+        <v>40</v>
+      </c>
+      <c r="J11" s="8">
+        <v>80</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="9">
+      <c r="B12" s="8">
         <v>110</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="8">
         <v>255</v>
       </c>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
+      <c r="D12" s="8">
+        <v>2</v>
+      </c>
+      <c r="E12" s="8">
+        <v>9.9</v>
+      </c>
+      <c r="F12" s="8">
+        <v>0</v>
+      </c>
+      <c r="G12" s="8">
+        <v>0</v>
+      </c>
+      <c r="H12" s="5">
+        <v>0</v>
+      </c>
+      <c r="I12" s="8">
+        <v>40</v>
+      </c>
+      <c r="J12" s="8">
+        <v>80</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="9">
+      <c r="B13" s="8">
         <v>70</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="8">
         <v>80</v>
       </c>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
+      <c r="D13" s="8">
+        <v>2</v>
+      </c>
+      <c r="E13" s="8">
+        <v>11.3</v>
+      </c>
+      <c r="F13" s="8">
+        <v>0</v>
+      </c>
+      <c r="G13" s="8">
+        <v>0</v>
+      </c>
+      <c r="H13" s="5">
+        <v>0</v>
+      </c>
+      <c r="I13" s="8">
+        <v>0</v>
+      </c>
+      <c r="J13" s="8">
+        <v>360</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="9">
-        <v>0</v>
-      </c>
-      <c r="C14" s="9">
-        <v>0</v>
-      </c>
-      <c r="D14" s="10"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
+      <c r="B14" s="8">
+        <v>0</v>
+      </c>
+      <c r="C14" s="8">
+        <v>0</v>
+      </c>
+      <c r="D14" s="9">
+        <v>0</v>
+      </c>
+      <c r="E14" s="8">
+        <v>7.1</v>
+      </c>
+      <c r="F14" s="8">
+        <v>0</v>
+      </c>
+      <c r="G14" s="8">
+        <v>0</v>
+      </c>
+      <c r="H14" s="8">
+        <v>500</v>
+      </c>
+      <c r="I14" s="8">
+        <v>0</v>
+      </c>
+      <c r="J14" s="8">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="9">
-        <v>0</v>
-      </c>
-      <c r="C15" s="9">
-        <v>0</v>
-      </c>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
+      <c r="B15" s="8">
+        <v>0</v>
+      </c>
+      <c r="C15" s="8">
+        <v>0</v>
+      </c>
+      <c r="D15" s="8">
+        <v>0</v>
+      </c>
+      <c r="E15" s="8">
+        <v>5</v>
+      </c>
+      <c r="F15" s="8">
+        <v>0</v>
+      </c>
+      <c r="G15" s="8">
+        <v>0</v>
+      </c>
+      <c r="H15" s="5">
+        <v>0</v>
+      </c>
+      <c r="I15" s="8">
+        <v>0</v>
+      </c>
+      <c r="J15" s="8">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="9">
-        <v>0</v>
-      </c>
-      <c r="C16" s="9">
-        <v>0</v>
-      </c>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
+      <c r="B16" s="8">
+        <v>0</v>
+      </c>
+      <c r="C16" s="8">
+        <v>0</v>
+      </c>
+      <c r="D16" s="8">
+        <v>0</v>
+      </c>
+      <c r="E16" s="8">
+        <v>5.7</v>
+      </c>
+      <c r="F16" s="8">
+        <v>0</v>
+      </c>
+      <c r="G16" s="8">
+        <v>5.6</v>
+      </c>
+      <c r="H16" s="5">
+        <v>0</v>
+      </c>
+      <c r="I16" s="8">
+        <v>0</v>
+      </c>
+      <c r="J16" s="8">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B17" s="9">
+      <c r="B17" s="8">
         <f>B11</f>
         <v>70</v>
       </c>
-      <c r="C17" s="9">
+      <c r="C17" s="8">
         <f>C11</f>
         <v>80</v>
       </c>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
+      <c r="D17" s="8">
+        <v>30</v>
+      </c>
+      <c r="E17" s="8">
+        <v>12</v>
+      </c>
+      <c r="F17" s="8">
+        <f>F9</f>
+        <v>16.5</v>
+      </c>
+      <c r="G17" s="8">
+        <v>0</v>
+      </c>
+      <c r="H17" s="5">
+        <v>0</v>
+      </c>
+      <c r="I17" s="8">
+        <v>10</v>
+      </c>
+      <c r="J17" s="8">
+        <v>20</v>
+      </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B18" s="9">
+      <c r="B18" s="8">
         <v>70</v>
       </c>
-      <c r="C18" s="9">
+      <c r="C18" s="8">
         <v>80</v>
       </c>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
+      <c r="D18" s="8">
+        <v>7</v>
+      </c>
+      <c r="E18" s="8">
+        <v>10.8</v>
+      </c>
+      <c r="F18" s="8">
+        <v>0</v>
+      </c>
+      <c r="G18" s="8">
+        <v>0</v>
+      </c>
+      <c r="H18" s="5">
+        <v>0</v>
+      </c>
+      <c r="I18" s="8">
+        <v>0</v>
+      </c>
+      <c r="J18" s="8">
+        <v>4</v>
+      </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B19" s="9">
+      <c r="B19" s="8">
         <v>70</v>
       </c>
-      <c r="C19" s="9">
+      <c r="C19" s="8">
         <v>80</v>
       </c>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
+      <c r="D19" s="8">
+        <v>2</v>
+      </c>
+      <c r="E19" s="8">
+        <v>6.9</v>
+      </c>
+      <c r="F19" s="8">
+        <v>0</v>
+      </c>
+      <c r="G19" s="8">
+        <v>0</v>
+      </c>
+      <c r="H19" s="5">
+        <v>0</v>
+      </c>
+      <c r="I19" s="8">
+        <v>0</v>
+      </c>
+      <c r="J19" s="8">
+        <v>4</v>
+      </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G22" s="13"/>
+      <c r="G22" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
shading properties of Singapore archetypes
- added shading type to construction archetypes
</commit_message>
<xml_diff>
--- a/cea/databases/archetypes/construction_properties_SIN.xlsx
+++ b/cea/databases/archetypes/construction_properties_SIN.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="61">
   <si>
     <t>Code</t>
   </si>
@@ -1102,7 +1102,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K17" sqref="K17"/>
+      <selection pane="bottomRight" activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1187,7 +1187,9 @@
       <c r="K2" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="L2" s="3"/>
+      <c r="L2" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="N2" s="11"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -1220,7 +1222,9 @@
       <c r="K3" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="L3" s="3"/>
+      <c r="L3" s="3" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
@@ -1252,7 +1256,9 @@
       <c r="K4" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="L4" s="3"/>
+      <c r="L4" s="3" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
@@ -1284,7 +1290,9 @@
       <c r="K5" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="L5" s="3"/>
+      <c r="L5" s="3" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
@@ -1316,7 +1324,9 @@
       <c r="K6" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="L6" s="3"/>
+      <c r="L6" s="3" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
@@ -1348,7 +1358,9 @@
       <c r="K7" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="L7" s="3"/>
+      <c r="L7" s="3" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
@@ -1380,7 +1392,9 @@
       <c r="K8" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="L8" s="3"/>
+      <c r="L8" s="3" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
@@ -1412,7 +1426,9 @@
       <c r="K9" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="L9" s="3"/>
+      <c r="L9" s="3" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
@@ -1444,7 +1460,9 @@
       <c r="K10" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="L10" s="3"/>
+      <c r="L10" s="3" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
@@ -1476,7 +1494,9 @@
       <c r="K11" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="L11" s="3"/>
+      <c r="L11" s="3" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
@@ -1508,7 +1528,9 @@
       <c r="K12" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="L12" s="3"/>
+      <c r="L12" s="3" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
@@ -1540,7 +1562,9 @@
       <c r="K13" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="L13" s="3"/>
+      <c r="L13" s="3" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
@@ -1572,7 +1596,9 @@
       <c r="K14" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="L14" s="3"/>
+      <c r="L14" s="3" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
@@ -1604,7 +1630,9 @@
       <c r="K15" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="L15" s="3"/>
+      <c r="L15" s="3" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
@@ -1636,7 +1664,9 @@
       <c r="K16" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="L16" s="3"/>
+      <c r="L16" s="3" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
@@ -1668,7 +1698,9 @@
       <c r="K17" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="L17" s="3"/>
+      <c r="L17" s="3" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
@@ -1700,7 +1732,9 @@
       <c r="K18" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="L18" s="3"/>
+      <c r="L18" s="3" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
@@ -1732,7 +1766,9 @@
       <c r="K19" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="L19" s="3"/>
+      <c r="L19" s="3" t="s">
+        <v>51</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added year to archetypes (only one construction per function for now)
- correction of Temperature set points to low values for no-heating
system case and high values for no-cooling system case (input has to be
double). I.e., can not be 'None' or 'NaN' or similar
</commit_message>
<xml_diff>
--- a/cea/databases/archetypes/construction_properties_SIN.xlsx
+++ b/cea/databases/archetypes/construction_properties_SIN.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="62">
   <si>
     <t>Code</t>
   </si>
@@ -203,9 +203,6 @@
     <t>T3</t>
   </si>
   <si>
-    <t>None</t>
-  </si>
-  <si>
     <t>T8</t>
   </si>
   <si>
@@ -213,6 +210,12 @@
   </si>
   <si>
     <t>T10</t>
+  </si>
+  <si>
+    <t>1950</t>
+  </si>
+  <si>
+    <t>2030</t>
   </si>
 </sst>
 </file>
@@ -1102,7 +1105,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L1" sqref="L1"/>
+      <selection pane="bottomRight" activeCell="B19" sqref="B19:C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1161,8 +1164,12 @@
       <c r="A2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
+      <c r="B2" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>61</v>
+      </c>
       <c r="D2" s="2" t="s">
         <v>48</v>
       </c>
@@ -1179,7 +1186,7 @@
         <v>56</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>53</v>
@@ -1196,8 +1203,12 @@
       <c r="A3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
+      <c r="B3" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>61</v>
+      </c>
       <c r="D3" s="2" t="s">
         <v>48</v>
       </c>
@@ -1214,7 +1225,7 @@
         <v>56</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>53</v>
@@ -1230,8 +1241,12 @@
       <c r="A4" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
+      <c r="B4" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>61</v>
+      </c>
       <c r="D4" s="2" t="s">
         <v>48</v>
       </c>
@@ -1248,7 +1263,7 @@
         <v>51</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>53</v>
@@ -1264,8 +1279,12 @@
       <c r="A5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
+      <c r="B5" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>61</v>
+      </c>
       <c r="D5" s="2" t="s">
         <v>48</v>
       </c>
@@ -1282,7 +1301,7 @@
         <v>51</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>53</v>
@@ -1298,8 +1317,12 @@
       <c r="A6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
+      <c r="B6" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>61</v>
+      </c>
       <c r="D6" s="2" t="s">
         <v>48</v>
       </c>
@@ -1316,7 +1339,7 @@
         <v>51</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J6" s="3" t="s">
         <v>53</v>
@@ -1332,8 +1355,12 @@
       <c r="A7" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
+      <c r="B7" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>61</v>
+      </c>
       <c r="D7" s="2" t="s">
         <v>48</v>
       </c>
@@ -1350,7 +1377,7 @@
         <v>51</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J7" s="3" t="s">
         <v>53</v>
@@ -1366,8 +1393,12 @@
       <c r="A8" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
+      <c r="B8" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>61</v>
+      </c>
       <c r="D8" s="2" t="s">
         <v>48</v>
       </c>
@@ -1384,7 +1415,7 @@
         <v>51</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J8" s="3" t="s">
         <v>53</v>
@@ -1400,8 +1431,12 @@
       <c r="A9" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
+      <c r="B9" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>61</v>
+      </c>
       <c r="D9" s="2" t="s">
         <v>48</v>
       </c>
@@ -1418,7 +1453,7 @@
         <v>51</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J9" s="3" t="s">
         <v>53</v>
@@ -1434,8 +1469,12 @@
       <c r="A10" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
+      <c r="B10" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>61</v>
+      </c>
       <c r="D10" s="2" t="s">
         <v>48</v>
       </c>
@@ -1452,7 +1491,7 @@
         <v>51</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J10" s="3" t="s">
         <v>53</v>
@@ -1468,8 +1507,12 @@
       <c r="A11" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
+      <c r="B11" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>61</v>
+      </c>
       <c r="D11" s="2" t="s">
         <v>48</v>
       </c>
@@ -1486,7 +1529,7 @@
         <v>51</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J11" s="3" t="s">
         <v>53</v>
@@ -1502,8 +1545,12 @@
       <c r="A12" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
+      <c r="B12" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>61</v>
+      </c>
       <c r="D12" s="2" t="s">
         <v>48</v>
       </c>
@@ -1520,7 +1567,7 @@
         <v>51</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J12" s="3" t="s">
         <v>53</v>
@@ -1536,8 +1583,12 @@
       <c r="A13" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
+      <c r="B13" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>61</v>
+      </c>
       <c r="D13" s="2" t="s">
         <v>48</v>
       </c>
@@ -1554,7 +1605,7 @@
         <v>51</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J13" s="3" t="s">
         <v>53</v>
@@ -1570,8 +1621,12 @@
       <c r="A14" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
+      <c r="B14" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>61</v>
+      </c>
       <c r="D14" s="2" t="s">
         <v>48</v>
       </c>
@@ -1588,7 +1643,7 @@
         <v>51</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J14" s="3" t="s">
         <v>53</v>
@@ -1604,8 +1659,12 @@
       <c r="A15" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
+      <c r="B15" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>61</v>
+      </c>
       <c r="D15" s="2" t="s">
         <v>48</v>
       </c>
@@ -1638,8 +1697,12 @@
       <c r="A16" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
+      <c r="B16" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>61</v>
+      </c>
       <c r="D16" s="2" t="s">
         <v>48</v>
       </c>
@@ -1672,8 +1735,12 @@
       <c r="A17" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
+      <c r="B17" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>61</v>
+      </c>
       <c r="D17" s="2" t="s">
         <v>48</v>
       </c>
@@ -1690,7 +1757,7 @@
         <v>51</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J17" s="3" t="s">
         <v>53</v>
@@ -1706,8 +1773,12 @@
       <c r="A18" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
+      <c r="B18" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>61</v>
+      </c>
       <c r="D18" s="2" t="s">
         <v>48</v>
       </c>
@@ -1724,7 +1795,7 @@
         <v>51</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J18" s="3" t="s">
         <v>53</v>
@@ -1740,8 +1811,12 @@
       <c r="A19" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
+      <c r="B19" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>61</v>
+      </c>
       <c r="D19" s="2" t="s">
         <v>48</v>
       </c>
@@ -1758,7 +1833,7 @@
         <v>51</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J19" s="3" t="s">
         <v>53</v>
@@ -1784,7 +1859,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H19" sqref="H19"/>
+      <selection pane="bottomRight" activeCell="B19" sqref="B19:C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1833,8 +1908,12 @@
       <c r="A2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
+      <c r="B2" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>61</v>
+      </c>
       <c r="D2" s="2" t="s">
         <v>48</v>
       </c>
@@ -1858,8 +1937,12 @@
       <c r="A3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
+      <c r="B3" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>61</v>
+      </c>
       <c r="D3" s="2" t="s">
         <v>48</v>
       </c>
@@ -1883,8 +1966,12 @@
       <c r="A4" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
+      <c r="B4" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>61</v>
+      </c>
       <c r="D4" s="2" t="s">
         <v>48</v>
       </c>
@@ -1908,8 +1995,12 @@
       <c r="A5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
+      <c r="B5" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>61</v>
+      </c>
       <c r="D5" s="2" t="s">
         <v>48</v>
       </c>
@@ -1933,8 +2024,12 @@
       <c r="A6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
+      <c r="B6" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>61</v>
+      </c>
       <c r="D6" s="2" t="s">
         <v>48</v>
       </c>
@@ -1958,8 +2053,12 @@
       <c r="A7" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
+      <c r="B7" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>61</v>
+      </c>
       <c r="D7" s="2" t="s">
         <v>48</v>
       </c>
@@ -1983,8 +2082,12 @@
       <c r="A8" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
+      <c r="B8" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>61</v>
+      </c>
       <c r="D8" s="2" t="s">
         <v>48</v>
       </c>
@@ -2008,8 +2111,12 @@
       <c r="A9" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
+      <c r="B9" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>61</v>
+      </c>
       <c r="D9" s="2" t="s">
         <v>48</v>
       </c>
@@ -2033,8 +2140,12 @@
       <c r="A10" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
+      <c r="B10" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>61</v>
+      </c>
       <c r="D10" s="2" t="s">
         <v>48</v>
       </c>
@@ -2058,8 +2169,12 @@
       <c r="A11" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
+      <c r="B11" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>61</v>
+      </c>
       <c r="D11" s="2" t="s">
         <v>48</v>
       </c>
@@ -2083,8 +2198,12 @@
       <c r="A12" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
+      <c r="B12" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>61</v>
+      </c>
       <c r="D12" s="2" t="s">
         <v>48</v>
       </c>
@@ -2108,8 +2227,12 @@
       <c r="A13" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
+      <c r="B13" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>61</v>
+      </c>
       <c r="D13" s="2" t="s">
         <v>48</v>
       </c>
@@ -2133,8 +2256,12 @@
       <c r="A14" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
+      <c r="B14" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>61</v>
+      </c>
       <c r="D14" s="2" t="s">
         <v>48</v>
       </c>
@@ -2158,8 +2285,12 @@
       <c r="A15" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
+      <c r="B15" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>61</v>
+      </c>
       <c r="D15" s="2" t="s">
         <v>48</v>
       </c>
@@ -2183,8 +2314,12 @@
       <c r="A16" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
+      <c r="B16" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>61</v>
+      </c>
       <c r="D16" s="2" t="s">
         <v>48</v>
       </c>
@@ -2208,8 +2343,12 @@
       <c r="A17" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
+      <c r="B17" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>61</v>
+      </c>
       <c r="D17" s="2" t="s">
         <v>48</v>
       </c>
@@ -2233,8 +2372,12 @@
       <c r="A18" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
+      <c r="B18" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>61</v>
+      </c>
       <c r="D18" s="2" t="s">
         <v>48</v>
       </c>
@@ -2258,8 +2401,12 @@
       <c r="A19" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
+      <c r="B19" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>61</v>
+      </c>
       <c r="D19" s="2" t="s">
         <v>48</v>
       </c>
@@ -2293,7 +2440,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F19"/>
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2334,14 +2481,14 @@
       <c r="B2" s="8">
         <v>24</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>57</v>
+      <c r="C2" s="5">
+        <v>10</v>
       </c>
       <c r="D2" s="8">
         <v>24</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>57</v>
+      <c r="E2" s="5">
+        <v>10</v>
       </c>
       <c r="F2" s="5">
         <v>10</v>
@@ -2354,14 +2501,14 @@
       <c r="B3" s="8">
         <v>24</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>57</v>
+      <c r="C3" s="5">
+        <v>10</v>
       </c>
       <c r="D3" s="8">
         <v>24</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>57</v>
+      <c r="E3" s="5">
+        <v>10</v>
       </c>
       <c r="F3" s="5">
         <v>10</v>
@@ -2374,14 +2521,14 @@
       <c r="B4" s="8">
         <v>24</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>57</v>
+      <c r="C4" s="5">
+        <v>10</v>
       </c>
       <c r="D4" s="8">
         <v>24</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>57</v>
+      <c r="E4" s="5">
+        <v>10</v>
       </c>
       <c r="F4" s="8">
         <v>10</v>
@@ -2394,14 +2541,14 @@
       <c r="B5" s="8">
         <v>24</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>57</v>
+      <c r="C5" s="5">
+        <v>10</v>
       </c>
       <c r="D5" s="3">
         <v>37</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>57</v>
+      <c r="E5" s="5">
+        <v>10</v>
       </c>
       <c r="F5" s="8">
         <v>10</v>
@@ -2414,14 +2561,14 @@
       <c r="B6" s="8">
         <v>24</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>57</v>
+      <c r="C6" s="5">
+        <v>10</v>
       </c>
       <c r="D6" s="3">
         <v>37</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>57</v>
+      <c r="E6" s="5">
+        <v>10</v>
       </c>
       <c r="F6" s="8">
         <v>8</v>
@@ -2434,14 +2581,14 @@
       <c r="B7" s="8">
         <v>24</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>57</v>
+      <c r="C7" s="5">
+        <v>10</v>
       </c>
       <c r="D7" s="8">
         <v>24</v>
       </c>
-      <c r="E7" s="5" t="s">
-        <v>57</v>
+      <c r="E7" s="5">
+        <v>10</v>
       </c>
       <c r="F7" s="8">
         <v>10</v>
@@ -2454,14 +2601,14 @@
       <c r="B8" s="8">
         <v>24</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>57</v>
+      <c r="C8" s="5">
+        <v>10</v>
       </c>
       <c r="D8" s="3">
         <v>37</v>
       </c>
-      <c r="E8" s="5" t="s">
-        <v>57</v>
+      <c r="E8" s="5">
+        <v>10</v>
       </c>
       <c r="F8" s="8">
         <f t="shared" ref="F8" si="0">111*0.15+10*0.85</f>
@@ -2475,14 +2622,14 @@
       <c r="B9" s="8">
         <v>24</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>57</v>
+      <c r="C9" s="5">
+        <v>10</v>
       </c>
       <c r="D9" s="3">
         <v>37</v>
       </c>
-      <c r="E9" s="5" t="s">
-        <v>57</v>
+      <c r="E9" s="5">
+        <v>10</v>
       </c>
       <c r="F9" s="8">
         <v>31</v>
@@ -2495,14 +2642,14 @@
       <c r="B10" s="8">
         <v>24</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>57</v>
+      <c r="C10" s="5">
+        <v>10</v>
       </c>
       <c r="D10" s="3">
         <v>37</v>
       </c>
-      <c r="E10" s="5" t="s">
-        <v>57</v>
+      <c r="E10" s="5">
+        <v>10</v>
       </c>
       <c r="F10" s="8">
         <v>8</v>
@@ -2515,14 +2662,14 @@
       <c r="B11" s="8">
         <v>24</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>57</v>
+      <c r="C11" s="5">
+        <v>10</v>
       </c>
       <c r="D11" s="8">
         <v>24</v>
       </c>
-      <c r="E11" s="5" t="s">
-        <v>57</v>
+      <c r="E11" s="5">
+        <v>10</v>
       </c>
       <c r="F11" s="8">
         <v>10</v>
@@ -2535,14 +2682,14 @@
       <c r="B12" s="8">
         <v>24</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>57</v>
+      <c r="C12" s="5">
+        <v>10</v>
       </c>
       <c r="D12" s="3">
         <v>37</v>
       </c>
-      <c r="E12" s="5" t="s">
-        <v>57</v>
+      <c r="E12" s="5">
+        <v>10</v>
       </c>
       <c r="F12" s="8">
         <v>10</v>
@@ -2552,17 +2699,17 @@
       <c r="A13" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>57</v>
+      <c r="B13" s="8">
+        <v>50</v>
+      </c>
+      <c r="C13" s="5">
+        <v>10</v>
+      </c>
+      <c r="D13" s="5">
+        <v>50</v>
+      </c>
+      <c r="E13" s="5">
+        <v>10</v>
       </c>
       <c r="F13" s="8">
         <v>36</v>
@@ -2575,14 +2722,14 @@
       <c r="B14" s="8">
         <v>24</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>57</v>
+      <c r="C14" s="5">
+        <v>10</v>
       </c>
       <c r="D14" s="8">
         <v>24</v>
       </c>
-      <c r="E14" s="5" t="s">
-        <v>57</v>
+      <c r="E14" s="5">
+        <v>10</v>
       </c>
       <c r="F14" s="8">
         <v>36</v>
@@ -2592,17 +2739,17 @@
       <c r="A15" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>57</v>
+      <c r="B15" s="8">
+        <v>50</v>
+      </c>
+      <c r="C15" s="5">
+        <v>10</v>
+      </c>
+      <c r="D15" s="5">
+        <v>50</v>
+      </c>
+      <c r="E15" s="5">
+        <v>10</v>
       </c>
       <c r="F15" s="8">
         <v>0</v>
@@ -2615,14 +2762,14 @@
       <c r="B16" s="8">
         <v>-5</v>
       </c>
-      <c r="C16" s="5" t="s">
-        <v>57</v>
+      <c r="C16" s="5">
+        <v>10</v>
       </c>
       <c r="D16" s="8">
         <v>-5</v>
       </c>
-      <c r="E16" s="5" t="s">
-        <v>57</v>
+      <c r="E16" s="5">
+        <v>10</v>
       </c>
       <c r="F16" s="8">
         <v>0</v>
@@ -2635,14 +2782,14 @@
       <c r="B17" s="8">
         <v>24</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>57</v>
+      <c r="C17" s="5">
+        <v>10</v>
       </c>
       <c r="D17" s="3">
         <v>37</v>
       </c>
-      <c r="E17" s="5" t="s">
-        <v>57</v>
+      <c r="E17" s="5">
+        <v>10</v>
       </c>
       <c r="F17" s="8">
         <f>F9</f>
@@ -2656,14 +2803,14 @@
       <c r="B18" s="8">
         <v>24</v>
       </c>
-      <c r="C18" s="5" t="s">
-        <v>57</v>
+      <c r="C18" s="5">
+        <v>10</v>
       </c>
       <c r="D18" s="3">
         <v>37</v>
       </c>
-      <c r="E18" s="5" t="s">
-        <v>57</v>
+      <c r="E18" s="5">
+        <v>10</v>
       </c>
       <c r="F18" s="8">
         <v>10</v>
@@ -2676,14 +2823,14 @@
       <c r="B19" s="8">
         <v>24</v>
       </c>
-      <c r="C19" s="5" t="s">
-        <v>57</v>
+      <c r="C19" s="5">
+        <v>10</v>
       </c>
       <c r="D19" s="3">
         <v>37</v>
       </c>
-      <c r="E19" s="5" t="s">
-        <v>57</v>
+      <c r="E19" s="5">
+        <v>10</v>
       </c>
       <c r="F19" s="8">
         <v>10</v>

</xml_diff>

<commit_message>
set start year of construction archetypes to 0
set start year of construction archetypes to 0, in order for buildings
with unknow age of construction(='1') to not cause properties script to
fail
</commit_message>
<xml_diff>
--- a/cea/databases/archetypes/construction_properties_SIN.xlsx
+++ b/cea/databases/archetypes/construction_properties_SIN.xlsx
@@ -212,10 +212,10 @@
     <t>T10</t>
   </si>
   <si>
-    <t>1950</t>
-  </si>
-  <si>
     <t>2030</t>
+  </si>
+  <si>
+    <t>0</t>
   </si>
 </sst>
 </file>
@@ -1105,7 +1105,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B19" sqref="B19:C19"/>
+      <selection pane="bottomRight" activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1165,10 +1165,10 @@
         <v>18</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>48</v>
@@ -1204,10 +1204,10 @@
         <v>19</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>48</v>
@@ -1242,10 +1242,10 @@
         <v>20</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>48</v>
@@ -1280,10 +1280,10 @@
         <v>21</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>48</v>
@@ -1318,10 +1318,10 @@
         <v>22</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>48</v>
@@ -1356,10 +1356,10 @@
         <v>32</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>48</v>
@@ -1394,10 +1394,10 @@
         <v>23</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>48</v>
@@ -1432,10 +1432,10 @@
         <v>24</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>48</v>
@@ -1470,10 +1470,10 @@
         <v>25</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>48</v>
@@ -1508,10 +1508,10 @@
         <v>26</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>48</v>
@@ -1546,10 +1546,10 @@
         <v>27</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>48</v>
@@ -1584,10 +1584,10 @@
         <v>28</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>48</v>
@@ -1622,10 +1622,10 @@
         <v>29</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>48</v>
@@ -1660,10 +1660,10 @@
         <v>30</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>48</v>
@@ -1698,10 +1698,10 @@
         <v>31</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>48</v>
@@ -1736,10 +1736,10 @@
         <v>41</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>48</v>
@@ -1774,10 +1774,10 @@
         <v>42</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>48</v>
@@ -1812,10 +1812,10 @@
         <v>43</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>48</v>
@@ -1859,7 +1859,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B19" sqref="B19:C19"/>
+      <selection pane="bottomRight" activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1909,10 +1909,10 @@
         <v>18</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>48</v>
@@ -1938,10 +1938,10 @@
         <v>19</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>48</v>
@@ -1967,10 +1967,10 @@
         <v>20</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>48</v>
@@ -1996,10 +1996,10 @@
         <v>21</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>48</v>
@@ -2025,10 +2025,10 @@
         <v>22</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>48</v>
@@ -2054,10 +2054,10 @@
         <v>32</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>48</v>
@@ -2083,10 +2083,10 @@
         <v>23</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>48</v>
@@ -2112,10 +2112,10 @@
         <v>24</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>48</v>
@@ -2141,10 +2141,10 @@
         <v>25</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>48</v>
@@ -2170,10 +2170,10 @@
         <v>26</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>48</v>
@@ -2199,10 +2199,10 @@
         <v>27</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>48</v>
@@ -2228,10 +2228,10 @@
         <v>28</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>48</v>
@@ -2257,10 +2257,10 @@
         <v>29</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>48</v>
@@ -2286,10 +2286,10 @@
         <v>30</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>48</v>
@@ -2315,10 +2315,10 @@
         <v>31</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>48</v>
@@ -2344,10 +2344,10 @@
         <v>41</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>48</v>
@@ -2373,10 +2373,10 @@
         <v>42</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>48</v>
@@ -2402,10 +2402,10 @@
         <v>43</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>48</v>

</xml_diff>

<commit_message>
Singapore process heating blank
The data in the Swiss construction archetypes was based on Swiss
statistics. Something similar should be done for Singapore as required.
</commit_message>
<xml_diff>
--- a/cea/databases/archetypes/construction_properties_SIN.xlsx
+++ b/cea/databases/archetypes/construction_properties_SIN.xlsx
@@ -17,7 +17,7 @@
     <sheet name="INDOOR_COMFORT" sheetId="6" r:id="rId3"/>
     <sheet name="INTERNAL_LOADS" sheetId="7" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
@@ -3033,7 +3033,7 @@
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="P40" sqref="P40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3386,7 +3386,7 @@
         <v>20</v>
       </c>
       <c r="K9" s="5">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="L9" s="5">
         <v>0</v>
@@ -3462,7 +3462,7 @@
         <v>80</v>
       </c>
       <c r="K11" s="5">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="L11" s="5">
         <v>0</v>

</xml_diff>

<commit_message>
overwriting new construction properties singapore
</commit_message>
<xml_diff>
--- a/cea/databases/archetypes/construction_properties_SIN.xlsx
+++ b/cea/databases/archetypes/construction_properties_SIN.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jimeno\Documents\CityEnergyAnalyst\cea\databases\archetypes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jimeno\Documents\CityEnergyAnalyst\cea\databases\SIN\archetypes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="458" windowWidth="38400" windowHeight="22020" tabRatio="785" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="458" windowWidth="38400" windowHeight="22020" tabRatio="785" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ARCHITECTURE" sheetId="3" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="69">
   <si>
     <t>Code</t>
   </si>
@@ -234,6 +234,9 @@
   </si>
   <si>
     <t>T4</t>
+  </si>
+  <si>
+    <t>UNIVERSITY</t>
   </si>
 </sst>
 </file>
@@ -1117,13 +1120,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q19"/>
+  <dimension ref="A1:Q20"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I24" sqref="I24"/>
+      <selection pane="bottomRight" activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1566,7 +1569,7 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A10" s="6" t="s">
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>60</v>
@@ -1599,7 +1602,7 @@
         <v>50</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="M10" s="3" t="s">
         <v>52</v>
@@ -1613,7 +1616,7 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A11" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>60</v>
@@ -1625,7 +1628,7 @@
         <v>47</v>
       </c>
       <c r="E11" s="3">
-        <v>0.84</v>
+        <v>0.67</v>
       </c>
       <c r="F11" s="3">
         <v>0.35</v>
@@ -1646,7 +1649,7 @@
         <v>50</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M11" s="3" t="s">
         <v>52</v>
@@ -1660,7 +1663,7 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A12" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>60</v>
@@ -1672,7 +1675,7 @@
         <v>47</v>
       </c>
       <c r="E12" s="3">
-        <v>0.67</v>
+        <v>0.84</v>
       </c>
       <c r="F12" s="3">
         <v>0.35</v>
@@ -1693,7 +1696,7 @@
         <v>50</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="M12" s="3" t="s">
         <v>52</v>
@@ -1707,7 +1710,7 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A13" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>60</v>
@@ -1719,7 +1722,7 @@
         <v>47</v>
       </c>
       <c r="E13" s="3">
-        <v>0</v>
+        <v>0.67</v>
       </c>
       <c r="F13" s="3">
         <v>0.35</v>
@@ -1740,21 +1743,21 @@
         <v>50</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M13" s="3" t="s">
         <v>52</v>
       </c>
       <c r="N13" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="O13" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A14" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>60</v>
@@ -1766,19 +1769,19 @@
         <v>47</v>
       </c>
       <c r="E14" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F14" s="3">
-        <v>0</v>
+        <v>0.35</v>
       </c>
       <c r="G14" s="3">
-        <v>0</v>
+        <v>0.35</v>
       </c>
       <c r="H14" s="3">
-        <v>0</v>
+        <v>0.35</v>
       </c>
       <c r="I14" s="3">
-        <v>0</v>
+        <v>0.35</v>
       </c>
       <c r="J14" s="3" t="s">
         <v>51</v>
@@ -1793,15 +1796,15 @@
         <v>52</v>
       </c>
       <c r="N14" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="O14" s="3" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A15" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>60</v>
@@ -1813,42 +1816,42 @@
         <v>47</v>
       </c>
       <c r="E15" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15" s="3">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G15" s="3">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="H15" s="3">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="I15" s="3">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="J15" s="3" t="s">
         <v>51</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="M15" s="3" t="s">
         <v>52</v>
       </c>
       <c r="N15" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="O15" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A16" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>60</v>
@@ -1860,25 +1863,25 @@
         <v>47</v>
       </c>
       <c r="E16" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F16" s="3">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G16" s="3">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H16" s="3">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I16" s="3">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="J16" s="3" t="s">
         <v>51</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="L16" s="3" t="s">
         <v>50</v>
@@ -1887,15 +1890,15 @@
         <v>52</v>
       </c>
       <c r="N16" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="O16" s="3" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A17" s="6" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>60</v>
@@ -1907,19 +1910,19 @@
         <v>47</v>
       </c>
       <c r="E17" s="3">
-        <v>0.67</v>
+        <v>1</v>
       </c>
       <c r="F17" s="3">
-        <v>0.35</v>
+        <v>0</v>
       </c>
       <c r="G17" s="3">
-        <v>0.35</v>
+        <v>0</v>
       </c>
       <c r="H17" s="3">
-        <v>0.35</v>
+        <v>0</v>
       </c>
       <c r="I17" s="3">
-        <v>0.35</v>
+        <v>0</v>
       </c>
       <c r="J17" s="3" t="s">
         <v>51</v>
@@ -1928,7 +1931,7 @@
         <v>50</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="M17" s="3" t="s">
         <v>52</v>
@@ -1942,7 +1945,7 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A18" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>60</v>
@@ -1989,7 +1992,7 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A19" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>60</v>
@@ -2031,12 +2034,62 @@
         <v>53</v>
       </c>
       <c r="O19" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A20" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E20" s="3">
+        <v>0.67</v>
+      </c>
+      <c r="F20" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="G20" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="H20" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="I20" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L20" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="M20" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="N20" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="O20" s="3" t="s">
         <v>50</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="B2:C20" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -2044,11 +2097,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K14" sqref="K14"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2326,8 +2376,8 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A10" s="6" t="s">
-        <v>24</v>
+      <c r="A10" s="7" t="s">
+        <v>68</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>60</v>
@@ -2356,7 +2406,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>60</v>
@@ -2374,7 +2424,7 @@
         <v>55</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>51</v>
@@ -2385,7 +2435,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>60</v>
@@ -2414,7 +2464,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>60</v>
@@ -2443,7 +2493,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>60</v>
@@ -2461,7 +2511,7 @@
         <v>55</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>51</v>
@@ -2472,7 +2522,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>60</v>
@@ -2487,21 +2537,21 @@
         <v>54</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>54</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>60</v>
@@ -2516,21 +2566,21 @@
         <v>54</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>54</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" s="6" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>60</v>
@@ -2548,7 +2598,7 @@
         <v>55</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>51</v>
@@ -2559,7 +2609,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>60</v>
@@ -2577,7 +2627,7 @@
         <v>55</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>51</v>
@@ -2588,7 +2638,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>60</v>
@@ -2612,6 +2662,35 @@
         <v>51</v>
       </c>
       <c r="I19" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A20" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I20" s="3" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2621,15 +2700,18 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="B2:C9 B10:C20" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2826,7 +2908,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="6" t="s">
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="B10" s="8">
         <v>24</v>
@@ -2841,12 +2923,12 @@
         <v>10</v>
       </c>
       <c r="F10" s="8">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" s="8">
         <v>24</v>
@@ -2854,19 +2936,19 @@
       <c r="C11" s="5">
         <v>10</v>
       </c>
-      <c r="D11" s="8">
-        <v>24</v>
+      <c r="D11" s="3">
+        <v>37</v>
       </c>
       <c r="E11" s="5">
         <v>10</v>
       </c>
       <c r="F11" s="8">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" s="8">
         <v>24</v>
@@ -2874,8 +2956,8 @@
       <c r="C12" s="5">
         <v>10</v>
       </c>
-      <c r="D12" s="3">
-        <v>37</v>
+      <c r="D12" s="8">
+        <v>24</v>
       </c>
       <c r="E12" s="5">
         <v>10</v>
@@ -2886,36 +2968,36 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" s="8">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="C13" s="5">
         <v>10</v>
       </c>
-      <c r="D13" s="5">
-        <v>50</v>
+      <c r="D13" s="3">
+        <v>37</v>
       </c>
       <c r="E13" s="5">
         <v>10</v>
       </c>
       <c r="F13" s="8">
-        <v>36</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14" s="8">
-        <v>24</v>
+        <v>50</v>
       </c>
       <c r="C14" s="5">
         <v>10</v>
       </c>
-      <c r="D14" s="8">
-        <v>24</v>
+      <c r="D14" s="5">
+        <v>50</v>
       </c>
       <c r="E14" s="5">
         <v>10</v>
@@ -2926,36 +3008,36 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B15" s="8">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="C15" s="5">
         <v>10</v>
       </c>
-      <c r="D15" s="5">
-        <v>50</v>
+      <c r="D15" s="8">
+        <v>24</v>
       </c>
       <c r="E15" s="5">
         <v>10</v>
       </c>
       <c r="F15" s="8">
-        <v>0</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B16" s="8">
-        <v>-5</v>
+        <v>50</v>
       </c>
       <c r="C16" s="5">
         <v>10</v>
       </c>
-      <c r="D16" s="8">
-        <v>-5</v>
+      <c r="D16" s="5">
+        <v>50</v>
       </c>
       <c r="E16" s="5">
         <v>10</v>
@@ -2966,48 +3048,48 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="8">
+        <v>-5</v>
+      </c>
+      <c r="C17" s="5">
+        <v>10</v>
+      </c>
+      <c r="D17" s="8">
+        <v>-5</v>
+      </c>
+      <c r="E17" s="5">
+        <v>10</v>
+      </c>
+      <c r="F17" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A18" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="8">
+      <c r="B18" s="8">
         <v>24</v>
       </c>
-      <c r="C17" s="5">
-        <v>10</v>
-      </c>
-      <c r="D17" s="3">
+      <c r="C18" s="5">
+        <v>10</v>
+      </c>
+      <c r="D18" s="3">
         <v>37</v>
       </c>
-      <c r="E17" s="5">
-        <v>10</v>
-      </c>
-      <c r="F17" s="8">
+      <c r="E18" s="5">
+        <v>10</v>
+      </c>
+      <c r="F18" s="8">
         <f>F9</f>
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A18" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B18" s="8">
-        <v>24</v>
-      </c>
-      <c r="C18" s="5">
-        <v>10</v>
-      </c>
-      <c r="D18" s="3">
-        <v>37</v>
-      </c>
-      <c r="E18" s="5">
-        <v>10</v>
-      </c>
-      <c r="F18" s="8">
-        <v>10</v>
-      </c>
-    </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B19" s="8">
         <v>24</v>
@@ -3022,6 +3104,26 @@
         <v>10</v>
       </c>
       <c r="F19" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A20" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="8">
+        <v>24</v>
+      </c>
+      <c r="C20" s="5">
+        <v>10</v>
+      </c>
+      <c r="D20" s="3">
+        <v>37</v>
+      </c>
+      <c r="E20" s="5">
+        <v>10</v>
+      </c>
+      <c r="F20" s="8">
         <v>10</v>
       </c>
     </row>
@@ -3033,10 +3135,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="P40" sqref="P40"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3398,7 +3500,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A10" s="6" t="s">
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="B10" s="8">
         <v>70</v>
@@ -3425,7 +3527,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="8">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="K10" s="5">
         <v>0</v>
@@ -3436,7 +3538,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A11" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" s="8">
         <v>70</v>
@@ -3445,10 +3547,10 @@
         <v>80</v>
       </c>
       <c r="D11" s="8">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E11" s="8">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F11" s="8">
         <v>0</v>
@@ -3460,10 +3562,10 @@
         <v>0</v>
       </c>
       <c r="I11" s="8">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="J11" s="8">
-        <v>80</v>
+        <v>4</v>
       </c>
       <c r="K11" s="5">
         <v>0</v>
@@ -3474,19 +3576,19 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A12" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" s="8">
-        <v>110</v>
+        <v>70</v>
       </c>
       <c r="C12" s="8">
-        <v>255</v>
+        <v>80</v>
       </c>
       <c r="D12" s="8">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E12" s="8">
-        <v>9.9</v>
+        <v>11</v>
       </c>
       <c r="F12" s="8">
         <v>0</v>
@@ -3498,7 +3600,7 @@
         <v>0</v>
       </c>
       <c r="I12" s="8">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="J12" s="8">
         <v>80</v>
@@ -3512,19 +3614,19 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A13" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" s="8">
-        <v>70</v>
+        <v>110</v>
       </c>
       <c r="C13" s="8">
-        <v>80</v>
+        <v>255</v>
       </c>
       <c r="D13" s="8">
         <v>2</v>
       </c>
       <c r="E13" s="8">
-        <v>11.3</v>
+        <v>9.9</v>
       </c>
       <c r="F13" s="8">
         <v>0</v>
@@ -3536,10 +3638,10 @@
         <v>0</v>
       </c>
       <c r="I13" s="8">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="J13" s="8">
-        <v>360</v>
+        <v>80</v>
       </c>
       <c r="K13" s="5">
         <v>0</v>
@@ -3550,19 +3652,19 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A14" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14" s="8">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="C14" s="8">
-        <v>0</v>
-      </c>
-      <c r="D14" s="9">
-        <v>0</v>
+        <v>80</v>
+      </c>
+      <c r="D14" s="8">
+        <v>2</v>
       </c>
       <c r="E14" s="8">
-        <v>7.1</v>
+        <v>11.3</v>
       </c>
       <c r="F14" s="8">
         <v>0</v>
@@ -3570,14 +3672,14 @@
       <c r="G14" s="8">
         <v>0</v>
       </c>
-      <c r="H14" s="8">
-        <v>500</v>
+      <c r="H14" s="5">
+        <v>0</v>
       </c>
       <c r="I14" s="8">
         <v>0</v>
       </c>
       <c r="J14" s="8">
-        <v>0</v>
+        <v>360</v>
       </c>
       <c r="K14" s="5">
         <v>0</v>
@@ -3588,7 +3690,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A15" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B15" s="8">
         <v>0</v>
@@ -3596,11 +3698,11 @@
       <c r="C15" s="8">
         <v>0</v>
       </c>
-      <c r="D15" s="8">
+      <c r="D15" s="9">
         <v>0</v>
       </c>
       <c r="E15" s="8">
-        <v>5</v>
+        <v>7.1</v>
       </c>
       <c r="F15" s="8">
         <v>0</v>
@@ -3608,8 +3710,8 @@
       <c r="G15" s="8">
         <v>0</v>
       </c>
-      <c r="H15" s="5">
-        <v>0</v>
+      <c r="H15" s="8">
+        <v>500</v>
       </c>
       <c r="I15" s="8">
         <v>0</v>
@@ -3626,7 +3728,7 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A16" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B16" s="8">
         <v>0</v>
@@ -3638,13 +3740,13 @@
         <v>0</v>
       </c>
       <c r="E16" s="8">
-        <v>5.7</v>
+        <v>5</v>
       </c>
       <c r="F16" s="8">
         <v>0</v>
       </c>
       <c r="G16" s="8">
-        <v>5.6</v>
+        <v>0</v>
       </c>
       <c r="H16" s="5">
         <v>0</v>
@@ -3664,75 +3766,75 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A17" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="8">
+        <v>0</v>
+      </c>
+      <c r="C17" s="8">
+        <v>0</v>
+      </c>
+      <c r="D17" s="8">
+        <v>0</v>
+      </c>
+      <c r="E17" s="8">
+        <v>5.7</v>
+      </c>
+      <c r="F17" s="8">
+        <v>0</v>
+      </c>
+      <c r="G17" s="8">
+        <v>5.6</v>
+      </c>
+      <c r="H17" s="5">
+        <v>0</v>
+      </c>
+      <c r="I17" s="8">
+        <v>0</v>
+      </c>
+      <c r="J17" s="8">
+        <v>0</v>
+      </c>
+      <c r="K17" s="5">
+        <v>0</v>
+      </c>
+      <c r="L17" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A18" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="8">
-        <f>B11</f>
+      <c r="B18" s="8">
+        <f>B12</f>
         <v>70</v>
       </c>
-      <c r="C17" s="8">
-        <f>C11</f>
+      <c r="C18" s="8">
+        <f>C12</f>
         <v>80</v>
       </c>
-      <c r="D17" s="8">
+      <c r="D18" s="8">
         <v>30</v>
       </c>
-      <c r="E17" s="8">
+      <c r="E18" s="8">
         <v>12</v>
       </c>
-      <c r="F17" s="8">
+      <c r="F18" s="8">
         <f>F9</f>
         <v>16.5</v>
       </c>
-      <c r="G17" s="8">
-        <v>0</v>
-      </c>
-      <c r="H17" s="5">
-        <v>0</v>
-      </c>
-      <c r="I17" s="8">
-        <v>10</v>
-      </c>
-      <c r="J17" s="8">
+      <c r="G18" s="8">
+        <v>0</v>
+      </c>
+      <c r="H18" s="5">
+        <v>0</v>
+      </c>
+      <c r="I18" s="8">
+        <v>10</v>
+      </c>
+      <c r="J18" s="8">
         <v>20</v>
-      </c>
-      <c r="K17" s="5">
-        <v>0</v>
-      </c>
-      <c r="L17" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A18" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B18" s="8">
-        <v>70</v>
-      </c>
-      <c r="C18" s="8">
-        <v>80</v>
-      </c>
-      <c r="D18" s="8">
-        <v>7</v>
-      </c>
-      <c r="E18" s="8">
-        <v>10.8</v>
-      </c>
-      <c r="F18" s="8">
-        <v>0</v>
-      </c>
-      <c r="G18" s="8">
-        <v>0</v>
-      </c>
-      <c r="H18" s="5">
-        <v>0</v>
-      </c>
-      <c r="I18" s="8">
-        <v>0</v>
-      </c>
-      <c r="J18" s="8">
-        <v>4</v>
       </c>
       <c r="K18" s="5">
         <v>0</v>
@@ -3743,7 +3845,7 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A19" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B19" s="8">
         <v>70</v>
@@ -3752,10 +3854,10 @@
         <v>80</v>
       </c>
       <c r="D19" s="8">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E19" s="8">
-        <v>6.9</v>
+        <v>10.8</v>
       </c>
       <c r="F19" s="8">
         <v>0</v>
@@ -3779,8 +3881,46 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="G22" s="12"/>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A20" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="8">
+        <v>70</v>
+      </c>
+      <c r="C20" s="8">
+        <v>80</v>
+      </c>
+      <c r="D20" s="8">
+        <v>2</v>
+      </c>
+      <c r="E20" s="8">
+        <v>6.9</v>
+      </c>
+      <c r="F20" s="8">
+        <v>0</v>
+      </c>
+      <c r="G20" s="8">
+        <v>0</v>
+      </c>
+      <c r="H20" s="5">
+        <v>0</v>
+      </c>
+      <c r="I20" s="8">
+        <v>0</v>
+      </c>
+      <c r="J20" s="8">
+        <v>4</v>
+      </c>
+      <c r="K20" s="5">
+        <v>0</v>
+      </c>
+      <c r="L20" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="G23" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>